<commit_message>
Changed hardcoded values from excel file
</commit_message>
<xml_diff>
--- a/7rSupermarketProject/src/test/resources/7rSuperMarketTestData.xlsx
+++ b/7rSupermarketProject/src/test/resources/7rSuperMarketTestData.xlsx
@@ -8,12 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\git\7rSuperMarket\7rSupermarketProject\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{433FB6D0-E94B-4305-9319-483CAFF75BF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00DE7E81-7154-42BC-8AA2-059AF30D8961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{616A25A6-6A29-4579-AAF8-0B1917F3D5F7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="6" xr2:uid="{616A25A6-6A29-4579-AAF8-0B1917F3D5F7}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginDetails" sheetId="1" r:id="rId1"/>
+    <sheet name="AdminUserDetails" sheetId="2" r:id="rId2"/>
+    <sheet name="CategoryDetail" sheetId="3" r:id="rId3"/>
+    <sheet name="ContactDetails" sheetId="4" r:id="rId4"/>
+    <sheet name="FooterDetails" sheetId="5" r:id="rId5"/>
+    <sheet name="NewDetails" sheetId="6" r:id="rId6"/>
+    <sheet name="SubCategoryDetails" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="28">
   <si>
     <t>UserName</t>
   </si>
@@ -46,16 +52,87 @@
   </si>
   <si>
     <t>akhil</t>
+  </si>
+  <si>
+    <t>AdminUserName</t>
+  </si>
+  <si>
+    <t>AdminPassword</t>
+  </si>
+  <si>
+    <t>Akhil</t>
+  </si>
+  <si>
+    <t>User123</t>
+  </si>
+  <si>
+    <t>CategoryName</t>
+  </si>
+  <si>
+    <t>Test Category 1122</t>
+  </si>
+  <si>
+    <t>PhoneNo</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Delivery Time</t>
+  </si>
+  <si>
+    <t>Delivery Charge</t>
+  </si>
+  <si>
+    <t>test1122@mail.com</t>
+  </si>
+  <si>
+    <t>Phase 1, Technopark</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Asiatic business center,Technopark Phase</t>
+  </si>
+  <si>
+    <t>testing@gmail.com</t>
+  </si>
+  <si>
+    <t>8947584758</t>
+  </si>
+  <si>
+    <t>News</t>
+  </si>
+  <si>
+    <t>Lorem Ipsum is simply dummy text of the printing and typesetting industry.</t>
+  </si>
+  <si>
+    <t>SubCategoryName</t>
+  </si>
+  <si>
+    <t>Test Subcategory 1126</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -78,13 +155,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -399,8 +480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0199C51E-DBD8-4834-B9CB-972F535973D5}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -452,4 +533,306 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{285AC2F9-66B9-4CE5-84D1-B4FABFEB1DB3}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="16.5546875" customWidth="1"/>
+    <col min="3" max="3" width="23.44140625" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93C61A79-05D2-428D-BEF0-30C9884FFEE0}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.44140625" customWidth="1"/>
+    <col min="2" max="2" width="10.88671875" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E3610D7-D404-4A22-B515-E6B6D665FBAB}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.109375" customWidth="1"/>
+    <col min="2" max="2" width="10.21875" customWidth="1"/>
+    <col min="3" max="3" width="25.109375" customWidth="1"/>
+    <col min="4" max="4" width="20.88671875" customWidth="1"/>
+    <col min="5" max="5" width="30.6640625" customWidth="1"/>
+    <col min="6" max="6" width="13.44140625" customWidth="1"/>
+    <col min="7" max="7" width="16.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>9995870445</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2">
+        <v>10</v>
+      </c>
+      <c r="G2">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{FB996CE7-73EB-48E2-AAA9-CF79073DEDD5}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D243CE62-D434-4DCC-A2F3-43E24F725B5A}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.5546875" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" customWidth="1"/>
+    <col min="3" max="3" width="45.5546875" customWidth="1"/>
+    <col min="4" max="4" width="22.109375" customWidth="1"/>
+    <col min="5" max="5" width="25.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{9DFEAAE2-8C43-461D-8A30-5706FBEC36D0}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E19CE0C-16A7-48C7-85FB-7E29A74E5F5E}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="68.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8BB6CB9-137E-4661-BBBA-89B0CC71A6F9}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="35.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
MultiBrowser,Parallel XML and Retry code updates
</commit_message>
<xml_diff>
--- a/7rSupermarketProject/src/test/resources/7rSuperMarketTestData.xlsx
+++ b/7rSupermarketProject/src/test/resources/7rSuperMarketTestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\git\7rSuperMarket\7rSupermarketProject\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00DE7E81-7154-42BC-8AA2-059AF30D8961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DA78FD7-1752-4CF0-948E-A99033EC553B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="6" xr2:uid="{616A25A6-6A29-4579-AAF8-0B1917F3D5F7}"/>
+    <workbookView xWindow="1488" yWindow="4020" windowWidth="21072" windowHeight="6960" xr2:uid="{616A25A6-6A29-4579-AAF8-0B1917F3D5F7}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginDetails" sheetId="1" r:id="rId1"/>
@@ -480,8 +480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0199C51E-DBD8-4834-B9CB-972F535973D5}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -801,7 +801,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8BB6CB9-137E-4661-BBBA-89B0CC71A6F9}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>

</xml_diff>